<commit_message>
added draft manual calibration for steady state model, including code to get around flopy error.  work-around still doesn't work properly, need to fix
</commit_message>
<xml_diff>
--- a/modflow_calibration/ss_calibration/ss_manual_calibration_log.xlsx
+++ b/modflow_calibration/ss_calibration/ss_manual_calibration_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\russian_river\model\RR_GSFLOW\modflow_calibration\ss_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F50BCAD-6697-4C1D-A999-91F88A192FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E02359-B73E-4067-85E4-4F02627E8584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13365" yWindow="3960" windowWidth="22815" windowHeight="13965" xr2:uid="{751A0CE8-76C8-4A3B-BE59-914A75BC760C}"/>
+    <workbookView xWindow="3795" yWindow="4965" windowWidth="21840" windowHeight="12855" xr2:uid="{751A0CE8-76C8-4A3B-BE59-914A75BC760C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Run ID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Lakebed leakance</t>
   </si>
   <si>
-    <t>Vertical K</t>
-  </si>
-  <si>
     <t>Rubber dam gate specified flow</t>
   </si>
   <si>
@@ -96,6 +93,21 @@
   </si>
   <si>
     <t>Rubber dam spillway specified width</t>
+  </si>
+  <si>
+    <t>07_20210603</t>
+  </si>
+  <si>
+    <t>increase lakebed leakance</t>
+  </si>
+  <si>
+    <t>08_20210603</t>
+  </si>
+  <si>
+    <t>Ks</t>
+  </si>
+  <si>
+    <t>increase Ks  for zone containing H0_23</t>
   </si>
 </sst>
 </file>
@@ -467,7 +479,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,22 +506,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
@@ -518,15 +530,15 @@
         <v>5</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>10.199999999999999</v>
@@ -553,18 +565,18 @@
         <v>11.3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>10.199999999999999</v>
@@ -591,18 +603,18 @@
         <v>11.2</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>10.199999999999999</v>
@@ -629,18 +641,18 @@
         <v>11.1</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>10.199999999999999</v>
@@ -667,18 +679,18 @@
         <v>14.3</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>10.199999999999999</v>
@@ -705,13 +717,83 @@
         <v>9.6</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D7">
+        <v>8.4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+      <c r="G7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I7">
+        <v>9.6</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D8">
+        <v>8.4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="G8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I8">
+        <v>9.6</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>